<commit_message>
feat: add words pairs to excel
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="188">
   <si>
     <t>English</t>
   </si>
@@ -55,15 +55,15 @@
     <t>Competitive programming</t>
   </si>
   <si>
+    <t>Until the end of time</t>
+  </si>
+  <si>
+    <t>Exception</t>
+  </si>
+  <si>
     <t>Word</t>
   </si>
   <si>
-    <t>Until the end of time</t>
-  </si>
-  <si>
-    <t>Exception</t>
-  </si>
-  <si>
     <t>Restore</t>
   </si>
   <si>
@@ -214,6 +214,99 @@
     <t>Book</t>
   </si>
   <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Specification</t>
+  </si>
+  <si>
+    <t>Responsibilities</t>
+  </si>
+  <si>
+    <t>Requirements</t>
+  </si>
+  <si>
+    <t>Reliable</t>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>Possible</t>
+  </si>
+  <si>
+    <t>Maintenance</t>
+  </si>
+  <si>
+    <t>Launch</t>
+  </si>
+  <si>
+    <t>Itemize</t>
+  </si>
+  <si>
+    <t>Indicate</t>
+  </si>
+  <si>
+    <t>Establish</t>
+  </si>
+  <si>
+    <t>Edit</t>
+  </si>
+  <si>
+    <t>Fix</t>
+  </si>
+  <si>
+    <t>Domain</t>
+  </si>
+  <si>
+    <t>Displayed</t>
+  </si>
+  <si>
+    <t>Discretion</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Cover</t>
+  </si>
+  <si>
+    <t>Content</t>
+  </si>
+  <si>
+    <t>Compatibility</t>
+  </si>
+  <si>
+    <t>Brief</t>
+  </si>
+  <si>
+    <t>Carefully</t>
+  </si>
+  <si>
+    <t>Beta test</t>
+  </si>
+  <si>
+    <t>Backup</t>
+  </si>
+  <si>
+    <t>Adjusted</t>
+  </si>
+  <si>
+    <t>Visual aids</t>
+  </si>
+  <si>
+    <t>Piace</t>
+  </si>
+  <si>
+    <t>Extra randomness</t>
+  </si>
+  <si>
+    <t>Check out the documentation</t>
+  </si>
+  <si>
+    <t>Multithreading</t>
+  </si>
+  <si>
     <t>Между частями приложения</t>
   </si>
   <si>
@@ -241,15 +334,15 @@
     <t>Конкурентное программирование</t>
   </si>
   <si>
+    <t>До конца веков</t>
+  </si>
+  <si>
+    <t>Исключение</t>
+  </si>
+  <si>
     <t>Слово</t>
   </si>
   <si>
-    <t>До конца веков</t>
-  </si>
-  <si>
-    <t>Исключение</t>
-  </si>
-  <si>
     <t>Восстанавливать</t>
   </si>
   <si>
@@ -395,6 +488,96 @@
   </si>
   <si>
     <t>Книга</t>
+  </si>
+  <si>
+    <t>Условие</t>
+  </si>
+  <si>
+    <t>Особенность</t>
+  </si>
+  <si>
+    <t>Обязанности</t>
+  </si>
+  <si>
+    <t>Требования</t>
+  </si>
+  <si>
+    <t>Надёжный</t>
+  </si>
+  <si>
+    <t>Возможный</t>
+  </si>
+  <si>
+    <t>Техобслуживание</t>
+  </si>
+  <si>
+    <t>Запуск</t>
+  </si>
+  <si>
+    <t>Составить перечень</t>
+  </si>
+  <si>
+    <t>Указать</t>
+  </si>
+  <si>
+    <t>Устанавливать</t>
+  </si>
+  <si>
+    <t>Редактировать</t>
+  </si>
+  <si>
+    <t>Исправлять</t>
+  </si>
+  <si>
+    <t>Домен</t>
+  </si>
+  <si>
+    <t>Отображаемый</t>
+  </si>
+  <si>
+    <t>Усмотрение</t>
+  </si>
+  <si>
+    <t>База данных</t>
+  </si>
+  <si>
+    <t>Описывать</t>
+  </si>
+  <si>
+    <t>Контент</t>
+  </si>
+  <si>
+    <t>Совместимость</t>
+  </si>
+  <si>
+    <t>Краткий</t>
+  </si>
+  <si>
+    <t>Тщательно</t>
+  </si>
+  <si>
+    <t>Опытная эксплуатация</t>
+  </si>
+  <si>
+    <t>Запас</t>
+  </si>
+  <si>
+    <t>Настроенный</t>
+  </si>
+  <si>
+    <t>Наглядные пособия</t>
+  </si>
+  <si>
+    <t>Мир</t>
+  </si>
+  <si>
+    <t>Лишняя случайность</t>
+  </si>
+  <si>
+    <t>Ознакомиться с документацией</t>
+  </si>
+  <si>
+    <t>Многопоточность</t>
   </si>
 </sst>
 </file>
@@ -752,7 +935,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B68"/>
+  <dimension ref="A1:B96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -771,7 +954,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>66</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -779,7 +962,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>98</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -787,7 +970,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -795,7 +978,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -803,7 +986,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>69</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -811,7 +994,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -819,7 +1002,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -827,7 +1010,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -835,7 +1018,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>72</v>
+        <v>103</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -843,7 +1026,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -851,7 +1034,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>74</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -859,447 +1042,671 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>75</v>
+        <v>107</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>75</v>
+        <v>108</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>76</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:2">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:2">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
     </row>
     <row r="22" spans="1:2">
       <c r="A22" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
     </row>
     <row r="23" spans="1:2">
       <c r="A23" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
     </row>
     <row r="24" spans="1:2">
       <c r="A24" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
     </row>
     <row r="25" spans="1:2">
       <c r="A25" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:2">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
     </row>
     <row r="34" spans="1:2">
       <c r="A34" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
     </row>
     <row r="35" spans="1:2">
       <c r="A35" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
     </row>
     <row r="36" spans="1:2">
       <c r="A36" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
     </row>
     <row r="38" spans="1:2">
       <c r="A38" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
     </row>
     <row r="39" spans="1:2">
       <c r="A39" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
     </row>
     <row r="40" spans="1:2">
       <c r="A40" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:2">
       <c r="A41" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:2">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:2">
       <c r="A44" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
     </row>
     <row r="45" spans="1:2">
       <c r="A45" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
     </row>
     <row r="47" spans="1:2">
       <c r="A47" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
     </row>
     <row r="48" spans="1:2">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
     </row>
     <row r="49" spans="1:2">
       <c r="A49" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
     </row>
     <row r="50" spans="1:2">
       <c r="A50" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>109</v>
+        <v>143</v>
       </c>
     </row>
     <row r="51" spans="1:2">
       <c r="A51" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>110</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:2">
       <c r="A52" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>111</v>
+        <v>145</v>
       </c>
     </row>
     <row r="53" spans="1:2">
       <c r="A53" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>112</v>
+        <v>146</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>113</v>
+        <v>147</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>149</v>
       </c>
     </row>
     <row r="57" spans="1:2">
       <c r="A57" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>116</v>
+        <v>150</v>
       </c>
     </row>
     <row r="58" spans="1:2">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>117</v>
+        <v>151</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>118</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>119</v>
+        <v>153</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>120</v>
+        <v>154</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>121</v>
+        <v>155</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>122</v>
+        <v>138</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>123</v>
+        <v>156</v>
       </c>
     </row>
     <row r="65" spans="1:2">
       <c r="A65" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>124</v>
+        <v>157</v>
       </c>
     </row>
     <row r="66" spans="1:2">
       <c r="A66" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>107</v>
+        <v>158</v>
       </c>
     </row>
     <row r="67" spans="1:2">
       <c r="A67" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>125</v>
+        <v>159</v>
       </c>
     </row>
     <row r="68" spans="1:2">
       <c r="A68" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>126</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>88</v>
+      </c>
+      <c r="B88" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>89</v>
+      </c>
+      <c r="B89" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>90</v>
+      </c>
+      <c r="B90" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>91</v>
+      </c>
+      <c r="B91" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>92</v>
+      </c>
+      <c r="B92" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>93</v>
+      </c>
+      <c r="B93" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>94</v>
+      </c>
+      <c r="B94" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>187</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel: add new pairs of words
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/WorkSpace/Home/Backend/Projects/Apps/Console_transtaler/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F617A-0ADB-1944-93B6-F538C4AC68A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="184">
   <si>
     <t>English</t>
   </si>
@@ -292,12 +298,6 @@
     <t>Adjusted</t>
   </si>
   <si>
-    <t>Visual aids</t>
-  </si>
-  <si>
-    <t>Piace</t>
-  </si>
-  <si>
     <t>Extra randomness</t>
   </si>
   <si>
@@ -563,12 +563,6 @@
   </si>
   <si>
     <t>Настроенный</t>
-  </si>
-  <si>
-    <t>Наглядные пособия</t>
-  </si>
-  <si>
-    <t>Мир</t>
   </si>
   <si>
     <t>Лишняя случайность</t>
@@ -583,8 +577,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -647,6 +641,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -693,7 +695,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -725,9 +727,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -759,6 +779,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -934,14 +972,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B96"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="C97" sqref="C97"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -949,764 +989,748 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2">
-      <c r="A95" t="s">
-        <v>95</v>
-      </c>
-      <c r="B95" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2">
-      <c r="A96" t="s">
-        <v>96</v>
-      </c>
-      <c r="B96" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
excel: add new pairs
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -1,26 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/WorkSpace/Home/Backend/Projects/Apps/Console_transtaler/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B37F617A-0ADB-1944-93B6-F538C4AC68A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="244">
   <si>
     <t>English</t>
   </si>
@@ -307,6 +301,96 @@
     <t>Multithreading</t>
   </si>
   <si>
+    <t>Visual aids</t>
+  </si>
+  <si>
+    <t>Totally</t>
+  </si>
+  <si>
+    <t>Sum up</t>
+  </si>
+  <si>
+    <t>Slightly</t>
+  </si>
+  <si>
+    <t>Share</t>
+  </si>
+  <si>
+    <t>Refer</t>
+  </si>
+  <si>
+    <t>Recap</t>
+  </si>
+  <si>
+    <t>Really</t>
+  </si>
+  <si>
+    <t>Quite</t>
+  </si>
+  <si>
+    <t>Properly</t>
+  </si>
+  <si>
+    <t>Outline</t>
+  </si>
+  <si>
+    <t>Obviously</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Move on</t>
+  </si>
+  <si>
+    <t>Mention</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Mainly</t>
+  </si>
+  <si>
+    <t>Likely</t>
+  </si>
+  <si>
+    <t>Instead</t>
+  </si>
+  <si>
+    <t>Extremely</t>
+  </si>
+  <si>
+    <t>Estimate</t>
+  </si>
+  <si>
+    <t>Especially</t>
+  </si>
+  <si>
+    <t>Directly</t>
+  </si>
+  <si>
+    <t>Deeply</t>
+  </si>
+  <si>
+    <t>Currently</t>
+  </si>
+  <si>
+    <t>Conclude</t>
+  </si>
+  <si>
+    <t>Completely</t>
+  </si>
+  <si>
+    <t>Briefly</t>
+  </si>
+  <si>
+    <t>Beg pardon</t>
+  </si>
+  <si>
+    <t>Acceptable</t>
+  </si>
+  <si>
     <t>Между частями приложения</t>
   </si>
   <si>
@@ -572,13 +656,103 @@
   </si>
   <si>
     <t>Многопоточность</t>
+  </si>
+  <si>
+    <t>Наглядные пособия</t>
+  </si>
+  <si>
+    <t>Полностью</t>
+  </si>
+  <si>
+    <t>Подводить итоги</t>
+  </si>
+  <si>
+    <t>Слегка</t>
+  </si>
+  <si>
+    <t>Делиться</t>
+  </si>
+  <si>
+    <t>Ссылаться</t>
+  </si>
+  <si>
+    <t>Резюмировать</t>
+  </si>
+  <si>
+    <t>Действительно</t>
+  </si>
+  <si>
+    <t>Довольно</t>
+  </si>
+  <si>
+    <t>Непосредственно</t>
+  </si>
+  <si>
+    <t>Очертить</t>
+  </si>
+  <si>
+    <t>Очевидно</t>
+  </si>
+  <si>
+    <t>Записи</t>
+  </si>
+  <si>
+    <t>Двигаться дальше</t>
+  </si>
+  <si>
+    <t>Упоминать</t>
+  </si>
+  <si>
+    <t>Иметь в виду</t>
+  </si>
+  <si>
+    <t>В основном</t>
+  </si>
+  <si>
+    <t>Похоже</t>
+  </si>
+  <si>
+    <t>Вместо</t>
+  </si>
+  <si>
+    <t>Сильно, интенсивно</t>
+  </si>
+  <si>
+    <t>Оценивать</t>
+  </si>
+  <si>
+    <t>Особенно</t>
+  </si>
+  <si>
+    <t>Напрямую</t>
+  </si>
+  <si>
+    <t>Детально</t>
+  </si>
+  <si>
+    <t>На данный момент</t>
+  </si>
+  <si>
+    <t>Сделать вывод</t>
+  </si>
+  <si>
+    <t>В полной мере</t>
+  </si>
+  <si>
+    <t>Кратко</t>
+  </si>
+  <si>
+    <t>Просить прощения</t>
+  </si>
+  <si>
+    <t>Приемлемый</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -641,14 +815,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -695,7 +861,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -727,27 +893,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -779,24 +927,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -972,16 +1102,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B94"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B124"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -989,748 +1117,988 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
       <c r="A94" t="s">
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>183</v>
+        <v>213</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>96</v>
+      </c>
+      <c r="B96" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>97</v>
+      </c>
+      <c r="B97" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>98</v>
+      </c>
+      <c r="B98" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>99</v>
+      </c>
+      <c r="B99" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>100</v>
+      </c>
+      <c r="B100" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>101</v>
+      </c>
+      <c r="B101" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2">
+      <c r="A102" t="s">
+        <v>102</v>
+      </c>
+      <c r="B102" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2">
+      <c r="A103" t="s">
+        <v>103</v>
+      </c>
+      <c r="B103" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2">
+      <c r="A104" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2">
+      <c r="A105" t="s">
+        <v>105</v>
+      </c>
+      <c r="B105" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2">
+      <c r="A106" t="s">
+        <v>106</v>
+      </c>
+      <c r="B106" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2">
+      <c r="A107" t="s">
+        <v>107</v>
+      </c>
+      <c r="B107" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2">
+      <c r="A108" t="s">
+        <v>108</v>
+      </c>
+      <c r="B108" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2">
+      <c r="A109" t="s">
+        <v>109</v>
+      </c>
+      <c r="B109" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2">
+      <c r="A110" t="s">
+        <v>110</v>
+      </c>
+      <c r="B110" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2">
+      <c r="A111" t="s">
+        <v>111</v>
+      </c>
+      <c r="B111" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2">
+      <c r="A112" t="s">
+        <v>112</v>
+      </c>
+      <c r="B112" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2">
+      <c r="A113" t="s">
+        <v>113</v>
+      </c>
+      <c r="B113" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2">
+      <c r="A114" t="s">
+        <v>114</v>
+      </c>
+      <c r="B114" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2">
+      <c r="A115" t="s">
+        <v>115</v>
+      </c>
+      <c r="B115" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2">
+      <c r="A116" t="s">
+        <v>116</v>
+      </c>
+      <c r="B116" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2">
+      <c r="A117" t="s">
+        <v>117</v>
+      </c>
+      <c r="B117" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2">
+      <c r="A118" t="s">
+        <v>118</v>
+      </c>
+      <c r="B118" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2">
+      <c r="A119" t="s">
+        <v>119</v>
+      </c>
+      <c r="B119" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="120" spans="1:2">
+      <c r="A120" t="s">
+        <v>120</v>
+      </c>
+      <c r="B120" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2">
+      <c r="A121" t="s">
+        <v>121</v>
+      </c>
+      <c r="B121" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2">
+      <c r="A122" t="s">
+        <v>122</v>
+      </c>
+      <c r="B122" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2">
+      <c r="A123" t="s">
+        <v>123</v>
+      </c>
+      <c r="B123" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2">
+      <c r="A124" t="s">
+        <v>124</v>
+      </c>
+      <c r="B124" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: Readme.md & add new pairs of words to excel
</commit_message>
<xml_diff>
--- a/words.xlsx
+++ b/words.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Documents/WorkSpace/Home/Backend/Projects/Apps/Console_transtaler/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D331E0-4AB4-BF4B-8894-4747C06D3C86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="500" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="848" uniqueCount="833">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="837">
   <si>
     <t>English</t>
   </si>
@@ -2513,13 +2519,25 @@
   </si>
   <si>
     <t>Унаследованное по</t>
+  </si>
+  <si>
+    <t>As soon as possible (asap)</t>
+  </si>
+  <si>
+    <t>Как можно скорее</t>
+  </si>
+  <si>
+    <t>Idle</t>
+  </si>
+  <si>
+    <t>Простой</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2582,6 +2600,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -2628,7 +2654,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2660,9 +2686,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2694,6 +2738,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2869,14 +2931,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B424"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B426"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A418" workbookViewId="0">
+      <selection activeCell="B419" sqref="B419"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="30" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2884,7 +2952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2892,7 +2960,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -2900,7 +2968,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -2908,7 +2976,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -2916,7 +2984,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -2924,7 +2992,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -2932,7 +3000,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -2940,7 +3008,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -2948,7 +3016,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -2956,7 +3024,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -2964,7 +3032,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -2972,7 +3040,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2980,7 +3048,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -2988,7 +3056,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>15</v>
       </c>
@@ -2996,7 +3064,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>16</v>
       </c>
@@ -3004,7 +3072,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -3012,7 +3080,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>18</v>
       </c>
@@ -3020,7 +3088,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>19</v>
       </c>
@@ -3028,7 +3096,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>20</v>
       </c>
@@ -3036,7 +3104,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>21</v>
       </c>
@@ -3044,7 +3112,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3052,7 +3120,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>23</v>
       </c>
@@ -3060,7 +3128,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>24</v>
       </c>
@@ -3068,7 +3136,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>25</v>
       </c>
@@ -3076,7 +3144,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>26</v>
       </c>
@@ -3084,7 +3152,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>27</v>
       </c>
@@ -3092,7 +3160,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>28</v>
       </c>
@@ -3100,7 +3168,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>29</v>
       </c>
@@ -3108,7 +3176,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>30</v>
       </c>
@@ -3116,7 +3184,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>31</v>
       </c>
@@ -3124,7 +3192,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>32</v>
       </c>
@@ -3132,7 +3200,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>33</v>
       </c>
@@ -3140,7 +3208,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>34</v>
       </c>
@@ -3148,7 +3216,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>35</v>
       </c>
@@ -3156,7 +3224,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>36</v>
       </c>
@@ -3164,7 +3232,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>37</v>
       </c>
@@ -3172,7 +3240,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>38</v>
       </c>
@@ -3180,7 +3248,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="39" spans="1:2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>39</v>
       </c>
@@ -3188,7 +3256,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>40</v>
       </c>
@@ -3196,7 +3264,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="41" spans="1:2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>41</v>
       </c>
@@ -3204,7 +3272,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>42</v>
       </c>
@@ -3212,7 +3280,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="43" spans="1:2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>43</v>
       </c>
@@ -3220,7 +3288,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>44</v>
       </c>
@@ -3228,7 +3296,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="45" spans="1:2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>45</v>
       </c>
@@ -3236,7 +3304,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>46</v>
       </c>
@@ -3244,7 +3312,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="47" spans="1:2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>47</v>
       </c>
@@ -3252,7 +3320,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>48</v>
       </c>
@@ -3260,7 +3328,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="49" spans="1:2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>49</v>
       </c>
@@ -3268,7 +3336,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>50</v>
       </c>
@@ -3276,7 +3344,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="51" spans="1:2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>51</v>
       </c>
@@ -3284,7 +3352,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>52</v>
       </c>
@@ -3292,7 +3360,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="53" spans="1:2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>53</v>
       </c>
@@ -3300,7 +3368,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="54" spans="1:2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -3308,7 +3376,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="55" spans="1:2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -3316,7 +3384,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="56" spans="1:2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -3324,7 +3392,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="57" spans="1:2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -3332,7 +3400,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="58" spans="1:2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -3340,7 +3408,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="59" spans="1:2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -3348,7 +3416,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="60" spans="1:2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -3356,7 +3424,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="61" spans="1:2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -3364,7 +3432,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="62" spans="1:2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -3372,7 +3440,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="63" spans="1:2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -3380,7 +3448,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="64" spans="1:2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -3388,7 +3456,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="65" spans="1:2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -3396,7 +3464,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="66" spans="1:2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -3404,7 +3472,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="67" spans="1:2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -3412,7 +3480,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="68" spans="1:2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -3420,7 +3488,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="69" spans="1:2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -3428,7 +3496,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="70" spans="1:2">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -3436,7 +3504,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="71" spans="1:2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -3444,7 +3512,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="72" spans="1:2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -3452,7 +3520,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="73" spans="1:2">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -3460,7 +3528,7 @@
         <v>490</v>
       </c>
     </row>
-    <row r="74" spans="1:2">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -3468,7 +3536,7 @@
         <v>491</v>
       </c>
     </row>
-    <row r="75" spans="1:2">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>75</v>
       </c>
@@ -3476,7 +3544,7 @@
         <v>492</v>
       </c>
     </row>
-    <row r="76" spans="1:2">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>76</v>
       </c>
@@ -3484,7 +3552,7 @@
         <v>493</v>
       </c>
     </row>
-    <row r="77" spans="1:2">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>77</v>
       </c>
@@ -3492,7 +3560,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="78" spans="1:2">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>78</v>
       </c>
@@ -3500,7 +3568,7 @@
         <v>495</v>
       </c>
     </row>
-    <row r="79" spans="1:2">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>79</v>
       </c>
@@ -3508,7 +3576,7 @@
         <v>496</v>
       </c>
     </row>
-    <row r="80" spans="1:2">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>80</v>
       </c>
@@ -3516,7 +3584,7 @@
         <v>497</v>
       </c>
     </row>
-    <row r="81" spans="1:2">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>81</v>
       </c>
@@ -3524,7 +3592,7 @@
         <v>498</v>
       </c>
     </row>
-    <row r="82" spans="1:2">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>82</v>
       </c>
@@ -3532,7 +3600,7 @@
         <v>499</v>
       </c>
     </row>
-    <row r="83" spans="1:2">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>83</v>
       </c>
@@ -3540,7 +3608,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="84" spans="1:2">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>84</v>
       </c>
@@ -3548,7 +3616,7 @@
         <v>501</v>
       </c>
     </row>
-    <row r="85" spans="1:2">
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>85</v>
       </c>
@@ -3556,7 +3624,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="86" spans="1:2">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>86</v>
       </c>
@@ -3564,7 +3632,7 @@
         <v>503</v>
       </c>
     </row>
-    <row r="87" spans="1:2">
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>87</v>
       </c>
@@ -3572,7 +3640,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="88" spans="1:2">
+    <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>88</v>
       </c>
@@ -3580,7 +3648,7 @@
         <v>505</v>
       </c>
     </row>
-    <row r="89" spans="1:2">
+    <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>89</v>
       </c>
@@ -3588,7 +3656,7 @@
         <v>506</v>
       </c>
     </row>
-    <row r="90" spans="1:2">
+    <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>90</v>
       </c>
@@ -3596,7 +3664,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="91" spans="1:2">
+    <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -3604,7 +3672,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="92" spans="1:2">
+    <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>92</v>
       </c>
@@ -3612,7 +3680,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="93" spans="1:2">
+    <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>93</v>
       </c>
@@ -3620,7 +3688,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="94" spans="1:2">
+    <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>94</v>
       </c>
@@ -3628,7 +3696,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="95" spans="1:2">
+    <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>95</v>
       </c>
@@ -3636,7 +3704,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="96" spans="1:2">
+    <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>96</v>
       </c>
@@ -3644,7 +3712,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="97" spans="1:2">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>97</v>
       </c>
@@ -3652,7 +3720,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="98" spans="1:2">
+    <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>98</v>
       </c>
@@ -3660,7 +3728,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="99" spans="1:2">
+    <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>99</v>
       </c>
@@ -3668,7 +3736,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="100" spans="1:2">
+    <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>100</v>
       </c>
@@ -3676,7 +3744,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="101" spans="1:2">
+    <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>101</v>
       </c>
@@ -3684,7 +3752,7 @@
         <v>518</v>
       </c>
     </row>
-    <row r="102" spans="1:2">
+    <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>102</v>
       </c>
@@ -3692,7 +3760,7 @@
         <v>519</v>
       </c>
     </row>
-    <row r="103" spans="1:2">
+    <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>103</v>
       </c>
@@ -3700,7 +3768,7 @@
         <v>520</v>
       </c>
     </row>
-    <row r="104" spans="1:2">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>104</v>
       </c>
@@ -3708,7 +3776,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="105" spans="1:2">
+    <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>105</v>
       </c>
@@ -3716,7 +3784,7 @@
         <v>522</v>
       </c>
     </row>
-    <row r="106" spans="1:2">
+    <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>106</v>
       </c>
@@ -3724,7 +3792,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="107" spans="1:2">
+    <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>107</v>
       </c>
@@ -3732,7 +3800,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="108" spans="1:2">
+    <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>108</v>
       </c>
@@ -3740,7 +3808,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="109" spans="1:2">
+    <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>109</v>
       </c>
@@ -3748,7 +3816,7 @@
         <v>526</v>
       </c>
     </row>
-    <row r="110" spans="1:2">
+    <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>110</v>
       </c>
@@ -3756,7 +3824,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="111" spans="1:2">
+    <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>111</v>
       </c>
@@ -3764,7 +3832,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="112" spans="1:2">
+    <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>112</v>
       </c>
@@ -3772,7 +3840,7 @@
         <v>529</v>
       </c>
     </row>
-    <row r="113" spans="1:2">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>113</v>
       </c>
@@ -3780,7 +3848,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="114" spans="1:2">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>114</v>
       </c>
@@ -3788,7 +3856,7 @@
         <v>531</v>
       </c>
     </row>
-    <row r="115" spans="1:2">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>115</v>
       </c>
@@ -3796,7 +3864,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="116" spans="1:2">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>116</v>
       </c>
@@ -3804,7 +3872,7 @@
         <v>533</v>
       </c>
     </row>
-    <row r="117" spans="1:2">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>117</v>
       </c>
@@ -3812,7 +3880,7 @@
         <v>534</v>
       </c>
     </row>
-    <row r="118" spans="1:2">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -3820,7 +3888,7 @@
         <v>535</v>
       </c>
     </row>
-    <row r="119" spans="1:2">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>119</v>
       </c>
@@ -3828,7 +3896,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="120" spans="1:2">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>120</v>
       </c>
@@ -3836,7 +3904,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="121" spans="1:2">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>121</v>
       </c>
@@ -3844,7 +3912,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="122" spans="1:2">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>122</v>
       </c>
@@ -3852,7 +3920,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="123" spans="1:2">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>123</v>
       </c>
@@ -3860,7 +3928,7 @@
         <v>540</v>
       </c>
     </row>
-    <row r="124" spans="1:2">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>124</v>
       </c>
@@ -3868,7 +3936,7 @@
         <v>541</v>
       </c>
     </row>
-    <row r="125" spans="1:2">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>125</v>
       </c>
@@ -3876,7 +3944,7 @@
         <v>542</v>
       </c>
     </row>
-    <row r="126" spans="1:2">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>126</v>
       </c>
@@ -3884,7 +3952,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="127" spans="1:2">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>127</v>
       </c>
@@ -3892,7 +3960,7 @@
         <v>544</v>
       </c>
     </row>
-    <row r="128" spans="1:2">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>128</v>
       </c>
@@ -3900,7 +3968,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="129" spans="1:2">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>129</v>
       </c>
@@ -3908,7 +3976,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="130" spans="1:2">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>130</v>
       </c>
@@ -3916,7 +3984,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="131" spans="1:2">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>131</v>
       </c>
@@ -3924,7 +3992,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="132" spans="1:2">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>132</v>
       </c>
@@ -3932,7 +4000,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="133" spans="1:2">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>133</v>
       </c>
@@ -3940,7 +4008,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="134" spans="1:2">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>134</v>
       </c>
@@ -3948,7 +4016,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="135" spans="1:2">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>135</v>
       </c>
@@ -3956,7 +4024,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="136" spans="1:2">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>136</v>
       </c>
@@ -3964,7 +4032,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="137" spans="1:2">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>137</v>
       </c>
@@ -3972,7 +4040,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="138" spans="1:2">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>138</v>
       </c>
@@ -3980,7 +4048,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="139" spans="1:2">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>139</v>
       </c>
@@ -3988,7 +4056,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="140" spans="1:2">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>140</v>
       </c>
@@ -3996,7 +4064,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="141" spans="1:2">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>141</v>
       </c>
@@ -4004,7 +4072,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="142" spans="1:2">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>142</v>
       </c>
@@ -4012,7 +4080,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="143" spans="1:2">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>143</v>
       </c>
@@ -4020,7 +4088,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="144" spans="1:2">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>144</v>
       </c>
@@ -4028,7 +4096,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="145" spans="1:2">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>145</v>
       </c>
@@ -4036,7 +4104,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="146" spans="1:2">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>146</v>
       </c>
@@ -4044,7 +4112,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="147" spans="1:2">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>147</v>
       </c>
@@ -4052,7 +4120,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="148" spans="1:2">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>148</v>
       </c>
@@ -4060,7 +4128,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="149" spans="1:2">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>149</v>
       </c>
@@ -4068,7 +4136,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="150" spans="1:2">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>150</v>
       </c>
@@ -4076,7 +4144,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="151" spans="1:2">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>151</v>
       </c>
@@ -4084,7 +4152,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="152" spans="1:2">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>152</v>
       </c>
@@ -4092,7 +4160,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="153" spans="1:2">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>153</v>
       </c>
@@ -4100,7 +4168,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="154" spans="1:2">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>154</v>
       </c>
@@ -4108,7 +4176,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="155" spans="1:2">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>155</v>
       </c>
@@ -4116,7 +4184,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="156" spans="1:2">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>156</v>
       </c>
@@ -4124,7 +4192,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="157" spans="1:2">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>157</v>
       </c>
@@ -4132,7 +4200,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="158" spans="1:2">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>158</v>
       </c>
@@ -4140,7 +4208,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="159" spans="1:2">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>159</v>
       </c>
@@ -4148,7 +4216,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="160" spans="1:2">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>160</v>
       </c>
@@ -4156,7 +4224,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="161" spans="1:2">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>161</v>
       </c>
@@ -4164,7 +4232,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="162" spans="1:2">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>162</v>
       </c>
@@ -4172,7 +4240,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="163" spans="1:2">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>163</v>
       </c>
@@ -4180,7 +4248,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="164" spans="1:2">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>164</v>
       </c>
@@ -4188,7 +4256,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="165" spans="1:2">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>165</v>
       </c>
@@ -4196,7 +4264,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="166" spans="1:2">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>166</v>
       </c>
@@ -4204,7 +4272,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="167" spans="1:2">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>167</v>
       </c>
@@ -4212,7 +4280,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="168" spans="1:2">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>168</v>
       </c>
@@ -4220,7 +4288,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="169" spans="1:2">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>169</v>
       </c>
@@ -4228,7 +4296,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="170" spans="1:2">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>170</v>
       </c>
@@ -4236,7 +4304,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="171" spans="1:2">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>171</v>
       </c>
@@ -4244,7 +4312,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="172" spans="1:2">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>172</v>
       </c>
@@ -4252,7 +4320,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="173" spans="1:2">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>173</v>
       </c>
@@ -4260,7 +4328,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="174" spans="1:2">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>174</v>
       </c>
@@ -4268,7 +4336,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="175" spans="1:2">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>175</v>
       </c>
@@ -4276,7 +4344,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="176" spans="1:2">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>176</v>
       </c>
@@ -4284,7 +4352,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="177" spans="1:2">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>177</v>
       </c>
@@ -4292,7 +4360,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="178" spans="1:2">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>178</v>
       </c>
@@ -4300,7 +4368,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="179" spans="1:2">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>179</v>
       </c>
@@ -4308,7 +4376,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="180" spans="1:2">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>180</v>
       </c>
@@ -4316,7 +4384,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="181" spans="1:2">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>181</v>
       </c>
@@ -4324,7 +4392,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="182" spans="1:2">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>182</v>
       </c>
@@ -4332,7 +4400,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="183" spans="1:2">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>183</v>
       </c>
@@ -4340,7 +4408,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="184" spans="1:2">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>184</v>
       </c>
@@ -4348,7 +4416,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="185" spans="1:2">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>185</v>
       </c>
@@ -4356,7 +4424,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="186" spans="1:2">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>186</v>
       </c>
@@ -4364,7 +4432,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="187" spans="1:2">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>187</v>
       </c>
@@ -4372,7 +4440,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="188" spans="1:2">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>188</v>
       </c>
@@ -4380,7 +4448,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="189" spans="1:2">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>189</v>
       </c>
@@ -4388,7 +4456,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="190" spans="1:2">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>190</v>
       </c>
@@ -4396,7 +4464,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="191" spans="1:2">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>191</v>
       </c>
@@ -4404,7 +4472,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="192" spans="1:2">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>192</v>
       </c>
@@ -4412,7 +4480,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="193" spans="1:2">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>193</v>
       </c>
@@ -4420,7 +4488,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="194" spans="1:2">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>194</v>
       </c>
@@ -4428,7 +4496,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="195" spans="1:2">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>195</v>
       </c>
@@ -4436,7 +4504,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="196" spans="1:2">
+    <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>196</v>
       </c>
@@ -4444,7 +4512,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="197" spans="1:2">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>197</v>
       </c>
@@ -4452,7 +4520,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="198" spans="1:2">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>198</v>
       </c>
@@ -4460,7 +4528,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="199" spans="1:2">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>199</v>
       </c>
@@ -4468,7 +4536,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="200" spans="1:2">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>200</v>
       </c>
@@ -4476,7 +4544,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="201" spans="1:2">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>201</v>
       </c>
@@ -4484,7 +4552,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="202" spans="1:2">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>202</v>
       </c>
@@ -4492,7 +4560,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="203" spans="1:2">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>203</v>
       </c>
@@ -4500,7 +4568,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="204" spans="1:2">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>204</v>
       </c>
@@ -4508,7 +4576,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="205" spans="1:2">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>205</v>
       </c>
@@ -4516,7 +4584,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="206" spans="1:2">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>206</v>
       </c>
@@ -4524,7 +4592,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="207" spans="1:2">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>207</v>
       </c>
@@ -4532,7 +4600,7 @@
         <v>623</v>
       </c>
     </row>
-    <row r="208" spans="1:2">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>208</v>
       </c>
@@ -4540,7 +4608,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="209" spans="1:2">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>209</v>
       </c>
@@ -4548,7 +4616,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="210" spans="1:2">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>210</v>
       </c>
@@ -4556,7 +4624,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="211" spans="1:2">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>211</v>
       </c>
@@ -4564,7 +4632,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="212" spans="1:2">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>212</v>
       </c>
@@ -4572,7 +4640,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="213" spans="1:2">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>213</v>
       </c>
@@ -4580,7 +4648,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="214" spans="1:2">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>214</v>
       </c>
@@ -4588,7 +4656,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="215" spans="1:2">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>215</v>
       </c>
@@ -4596,7 +4664,7 @@
         <v>631</v>
       </c>
     </row>
-    <row r="216" spans="1:2">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>216</v>
       </c>
@@ -4604,7 +4672,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="217" spans="1:2">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>217</v>
       </c>
@@ -4612,7 +4680,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="218" spans="1:2">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>218</v>
       </c>
@@ -4620,7 +4688,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="219" spans="1:2">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>219</v>
       </c>
@@ -4628,7 +4696,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="220" spans="1:2">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>220</v>
       </c>
@@ -4636,7 +4704,7 @@
         <v>636</v>
       </c>
     </row>
-    <row r="221" spans="1:2">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>221</v>
       </c>
@@ -4644,7 +4712,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="222" spans="1:2">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>222</v>
       </c>
@@ -4652,7 +4720,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="223" spans="1:2">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>223</v>
       </c>
@@ -4660,7 +4728,7 @@
         <v>639</v>
       </c>
     </row>
-    <row r="224" spans="1:2">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>224</v>
       </c>
@@ -4668,7 +4736,7 @@
         <v>640</v>
       </c>
     </row>
-    <row r="225" spans="1:2">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>225</v>
       </c>
@@ -4676,7 +4744,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="226" spans="1:2">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>226</v>
       </c>
@@ -4684,7 +4752,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="227" spans="1:2">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>227</v>
       </c>
@@ -4692,7 +4760,7 @@
         <v>643</v>
       </c>
     </row>
-    <row r="228" spans="1:2">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>228</v>
       </c>
@@ -4700,7 +4768,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="229" spans="1:2">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>229</v>
       </c>
@@ -4708,7 +4776,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="230" spans="1:2">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>230</v>
       </c>
@@ -4716,7 +4784,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="231" spans="1:2">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>231</v>
       </c>
@@ -4724,7 +4792,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="232" spans="1:2">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>232</v>
       </c>
@@ -4732,7 +4800,7 @@
         <v>645</v>
       </c>
     </row>
-    <row r="233" spans="1:2">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>233</v>
       </c>
@@ -4740,7 +4808,7 @@
         <v>646</v>
       </c>
     </row>
-    <row r="234" spans="1:2">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>234</v>
       </c>
@@ -4748,7 +4816,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="235" spans="1:2">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>235</v>
       </c>
@@ -4756,7 +4824,7 @@
         <v>648</v>
       </c>
     </row>
-    <row r="236" spans="1:2">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>236</v>
       </c>
@@ -4764,7 +4832,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="237" spans="1:2">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>237</v>
       </c>
@@ -4772,7 +4840,7 @@
         <v>650</v>
       </c>
     </row>
-    <row r="238" spans="1:2">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>238</v>
       </c>
@@ -4780,7 +4848,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="239" spans="1:2">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>239</v>
       </c>
@@ -4788,7 +4856,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="240" spans="1:2">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>240</v>
       </c>
@@ -4796,7 +4864,7 @@
         <v>653</v>
       </c>
     </row>
-    <row r="241" spans="1:2">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>241</v>
       </c>
@@ -4804,7 +4872,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="242" spans="1:2">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>242</v>
       </c>
@@ -4812,7 +4880,7 @@
         <v>655</v>
       </c>
     </row>
-    <row r="243" spans="1:2">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>243</v>
       </c>
@@ -4820,7 +4888,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="244" spans="1:2">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>244</v>
       </c>
@@ -4828,7 +4896,7 @@
         <v>657</v>
       </c>
     </row>
-    <row r="245" spans="1:2">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>245</v>
       </c>
@@ -4836,7 +4904,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="246" spans="1:2">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>246</v>
       </c>
@@ -4844,7 +4912,7 @@
         <v>659</v>
       </c>
     </row>
-    <row r="247" spans="1:2">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>247</v>
       </c>
@@ -4852,7 +4920,7 @@
         <v>660</v>
       </c>
     </row>
-    <row r="248" spans="1:2">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>248</v>
       </c>
@@ -4860,7 +4928,7 @@
         <v>661</v>
       </c>
     </row>
-    <row r="249" spans="1:2">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>249</v>
       </c>
@@ -4868,7 +4936,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="250" spans="1:2">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>250</v>
       </c>
@@ -4876,7 +4944,7 @@
         <v>663</v>
       </c>
     </row>
-    <row r="251" spans="1:2">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>251</v>
       </c>
@@ -4884,7 +4952,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="252" spans="1:2">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>252</v>
       </c>
@@ -4892,7 +4960,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="253" spans="1:2">
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>253</v>
       </c>
@@ -4900,7 +4968,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="254" spans="1:2">
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>254</v>
       </c>
@@ -4908,7 +4976,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="255" spans="1:2">
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>255</v>
       </c>
@@ -4916,7 +4984,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="256" spans="1:2">
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>256</v>
       </c>
@@ -4924,7 +4992,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="257" spans="1:2">
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>257</v>
       </c>
@@ -4932,7 +5000,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="258" spans="1:2">
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>258</v>
       </c>
@@ -4940,7 +5008,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="259" spans="1:2">
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>259</v>
       </c>
@@ -4948,7 +5016,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="260" spans="1:2">
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>260</v>
       </c>
@@ -4956,7 +5024,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="261" spans="1:2">
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>261</v>
       </c>
@@ -4964,7 +5032,7 @@
         <v>674</v>
       </c>
     </row>
-    <row r="262" spans="1:2">
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>262</v>
       </c>
@@ -4972,7 +5040,7 @@
         <v>675</v>
       </c>
     </row>
-    <row r="263" spans="1:2">
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>263</v>
       </c>
@@ -4980,7 +5048,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="264" spans="1:2">
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>264</v>
       </c>
@@ -4988,7 +5056,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="265" spans="1:2">
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>265</v>
       </c>
@@ -4996,7 +5064,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="266" spans="1:2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>266</v>
       </c>
@@ -5004,7 +5072,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="267" spans="1:2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>267</v>
       </c>
@@ -5012,7 +5080,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="268" spans="1:2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>268</v>
       </c>
@@ -5020,7 +5088,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="269" spans="1:2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>269</v>
       </c>
@@ -5028,7 +5096,7 @@
         <v>681</v>
       </c>
     </row>
-    <row r="270" spans="1:2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>270</v>
       </c>
@@ -5036,7 +5104,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="271" spans="1:2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>271</v>
       </c>
@@ -5044,7 +5112,7 @@
         <v>682</v>
       </c>
     </row>
-    <row r="272" spans="1:2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>272</v>
       </c>
@@ -5052,7 +5120,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="273" spans="1:2">
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>273</v>
       </c>
@@ -5060,7 +5128,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="274" spans="1:2">
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>274</v>
       </c>
@@ -5068,7 +5136,7 @@
         <v>685</v>
       </c>
     </row>
-    <row r="275" spans="1:2">
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>275</v>
       </c>
@@ -5076,7 +5144,7 @@
         <v>686</v>
       </c>
     </row>
-    <row r="276" spans="1:2">
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>276</v>
       </c>
@@ -5084,7 +5152,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="277" spans="1:2">
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>277</v>
       </c>
@@ -5092,7 +5160,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="278" spans="1:2">
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>278</v>
       </c>
@@ -5100,7 +5168,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="279" spans="1:2">
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>279</v>
       </c>
@@ -5108,7 +5176,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="280" spans="1:2">
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>280</v>
       </c>
@@ -5116,7 +5184,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="281" spans="1:2">
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>194</v>
       </c>
@@ -5124,7 +5192,7 @@
         <v>692</v>
       </c>
     </row>
-    <row r="282" spans="1:2">
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>281</v>
       </c>
@@ -5132,7 +5200,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="283" spans="1:2">
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>282</v>
       </c>
@@ -5140,7 +5208,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="284" spans="1:2">
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>283</v>
       </c>
@@ -5148,7 +5216,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="285" spans="1:2">
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>284</v>
       </c>
@@ -5156,7 +5224,7 @@
         <v>696</v>
       </c>
     </row>
-    <row r="286" spans="1:2">
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>285</v>
       </c>
@@ -5164,7 +5232,7 @@
         <v>697</v>
       </c>
     </row>
-    <row r="287" spans="1:2">
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>286</v>
       </c>
@@ -5172,7 +5240,7 @@
         <v>698</v>
       </c>
     </row>
-    <row r="288" spans="1:2">
+    <row r="288" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>287</v>
       </c>
@@ -5180,7 +5248,7 @@
         <v>699</v>
       </c>
     </row>
-    <row r="289" spans="1:2">
+    <row r="289" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>288</v>
       </c>
@@ -5188,7 +5256,7 @@
         <v>700</v>
       </c>
     </row>
-    <row r="290" spans="1:2">
+    <row r="290" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>289</v>
       </c>
@@ -5196,7 +5264,7 @@
         <v>701</v>
       </c>
     </row>
-    <row r="291" spans="1:2">
+    <row r="291" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>290</v>
       </c>
@@ -5204,7 +5272,7 @@
         <v>702</v>
       </c>
     </row>
-    <row r="292" spans="1:2">
+    <row r="292" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>291</v>
       </c>
@@ -5212,7 +5280,7 @@
         <v>703</v>
       </c>
     </row>
-    <row r="293" spans="1:2">
+    <row r="293" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>292</v>
       </c>
@@ -5220,7 +5288,7 @@
         <v>704</v>
       </c>
     </row>
-    <row r="294" spans="1:2">
+    <row r="294" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>293</v>
       </c>
@@ -5228,7 +5296,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="295" spans="1:2">
+    <row r="295" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>294</v>
       </c>
@@ -5236,7 +5304,7 @@
         <v>706</v>
       </c>
     </row>
-    <row r="296" spans="1:2">
+    <row r="296" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>295</v>
       </c>
@@ -5244,7 +5312,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="297" spans="1:2">
+    <row r="297" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>296</v>
       </c>
@@ -5252,7 +5320,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="298" spans="1:2">
+    <row r="298" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>297</v>
       </c>
@@ -5260,7 +5328,7 @@
         <v>709</v>
       </c>
     </row>
-    <row r="299" spans="1:2">
+    <row r="299" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>298</v>
       </c>
@@ -5268,7 +5336,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="300" spans="1:2">
+    <row r="300" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>299</v>
       </c>
@@ -5276,7 +5344,7 @@
         <v>711</v>
       </c>
     </row>
-    <row r="301" spans="1:2">
+    <row r="301" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>300</v>
       </c>
@@ -5284,7 +5352,7 @@
         <v>712</v>
       </c>
     </row>
-    <row r="302" spans="1:2">
+    <row r="302" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>301</v>
       </c>
@@ -5292,7 +5360,7 @@
         <v>713</v>
       </c>
     </row>
-    <row r="303" spans="1:2">
+    <row r="303" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>302</v>
       </c>
@@ -5300,7 +5368,7 @@
         <v>714</v>
       </c>
     </row>
-    <row r="304" spans="1:2">
+    <row r="304" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>303</v>
       </c>
@@ -5308,7 +5376,7 @@
         <v>715</v>
       </c>
     </row>
-    <row r="305" spans="1:2">
+    <row r="305" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>304</v>
       </c>
@@ -5316,7 +5384,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="306" spans="1:2">
+    <row r="306" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>305</v>
       </c>
@@ -5324,7 +5392,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="307" spans="1:2">
+    <row r="307" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>306</v>
       </c>
@@ -5332,7 +5400,7 @@
         <v>718</v>
       </c>
     </row>
-    <row r="308" spans="1:2">
+    <row r="308" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>307</v>
       </c>
@@ -5340,7 +5408,7 @@
         <v>719</v>
       </c>
     </row>
-    <row r="309" spans="1:2">
+    <row r="309" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>308</v>
       </c>
@@ -5348,7 +5416,7 @@
         <v>720</v>
       </c>
     </row>
-    <row r="310" spans="1:2">
+    <row r="310" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>309</v>
       </c>
@@ -5356,7 +5424,7 @@
         <v>721</v>
       </c>
     </row>
-    <row r="311" spans="1:2">
+    <row r="311" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>310</v>
       </c>
@@ -5364,7 +5432,7 @@
         <v>722</v>
       </c>
     </row>
-    <row r="312" spans="1:2">
+    <row r="312" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>311</v>
       </c>
@@ -5372,7 +5440,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="313" spans="1:2">
+    <row r="313" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>312</v>
       </c>
@@ -5380,7 +5448,7 @@
         <v>724</v>
       </c>
     </row>
-    <row r="314" spans="1:2">
+    <row r="314" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>313</v>
       </c>
@@ -5388,7 +5456,7 @@
         <v>725</v>
       </c>
     </row>
-    <row r="315" spans="1:2">
+    <row r="315" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>314</v>
       </c>
@@ -5396,7 +5464,7 @@
         <v>726</v>
       </c>
     </row>
-    <row r="316" spans="1:2">
+    <row r="316" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>315</v>
       </c>
@@ -5404,7 +5472,7 @@
         <v>727</v>
       </c>
     </row>
-    <row r="317" spans="1:2">
+    <row r="317" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>316</v>
       </c>
@@ -5412,7 +5480,7 @@
         <v>728</v>
       </c>
     </row>
-    <row r="318" spans="1:2">
+    <row r="318" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>317</v>
       </c>
@@ -5420,7 +5488,7 @@
         <v>729</v>
       </c>
     </row>
-    <row r="319" spans="1:2">
+    <row r="319" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>318</v>
       </c>
@@ -5428,7 +5496,7 @@
         <v>730</v>
       </c>
     </row>
-    <row r="320" spans="1:2">
+    <row r="320" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>319</v>
       </c>
@@ -5436,7 +5504,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="321" spans="1:2">
+    <row r="321" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>320</v>
       </c>
@@ -5444,7 +5512,7 @@
         <v>732</v>
       </c>
     </row>
-    <row r="322" spans="1:2">
+    <row r="322" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>321</v>
       </c>
@@ -5452,7 +5520,7 @@
         <v>733</v>
       </c>
     </row>
-    <row r="323" spans="1:2">
+    <row r="323" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>322</v>
       </c>
@@ -5460,7 +5528,7 @@
         <v>734</v>
       </c>
     </row>
-    <row r="324" spans="1:2">
+    <row r="324" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>323</v>
       </c>
@@ -5468,7 +5536,7 @@
         <v>735</v>
       </c>
     </row>
-    <row r="325" spans="1:2">
+    <row r="325" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>324</v>
       </c>
@@ -5476,7 +5544,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="326" spans="1:2">
+    <row r="326" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>325</v>
       </c>
@@ -5484,7 +5552,7 @@
         <v>737</v>
       </c>
     </row>
-    <row r="327" spans="1:2">
+    <row r="327" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>326</v>
       </c>
@@ -5492,7 +5560,7 @@
         <v>738</v>
       </c>
     </row>
-    <row r="328" spans="1:2">
+    <row r="328" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>327</v>
       </c>
@@ -5500,7 +5568,7 @@
         <v>739</v>
       </c>
     </row>
-    <row r="329" spans="1:2">
+    <row r="329" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>328</v>
       </c>
@@ -5508,7 +5576,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="330" spans="1:2">
+    <row r="330" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>329</v>
       </c>
@@ -5516,7 +5584,7 @@
         <v>741</v>
       </c>
     </row>
-    <row r="331" spans="1:2">
+    <row r="331" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>330</v>
       </c>
@@ -5524,7 +5592,7 @@
         <v>742</v>
       </c>
     </row>
-    <row r="332" spans="1:2">
+    <row r="332" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>331</v>
       </c>
@@ -5532,7 +5600,7 @@
         <v>743</v>
       </c>
     </row>
-    <row r="333" spans="1:2">
+    <row r="333" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>332</v>
       </c>
@@ -5540,7 +5608,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="334" spans="1:2">
+    <row r="334" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>333</v>
       </c>
@@ -5548,7 +5616,7 @@
         <v>745</v>
       </c>
     </row>
-    <row r="335" spans="1:2">
+    <row r="335" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>334</v>
       </c>
@@ -5556,7 +5624,7 @@
         <v>746</v>
       </c>
     </row>
-    <row r="336" spans="1:2">
+    <row r="336" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>335</v>
       </c>
@@ -5564,7 +5632,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="337" spans="1:2">
+    <row r="337" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>336</v>
       </c>
@@ -5572,7 +5640,7 @@
         <v>748</v>
       </c>
     </row>
-    <row r="338" spans="1:2">
+    <row r="338" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>337</v>
       </c>
@@ -5580,7 +5648,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="339" spans="1:2">
+    <row r="339" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>338</v>
       </c>
@@ -5588,7 +5656,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="340" spans="1:2">
+    <row r="340" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>339</v>
       </c>
@@ -5596,7 +5664,7 @@
         <v>751</v>
       </c>
     </row>
-    <row r="341" spans="1:2">
+    <row r="341" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>340</v>
       </c>
@@ -5604,7 +5672,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="342" spans="1:2">
+    <row r="342" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>341</v>
       </c>
@@ -5612,7 +5680,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="343" spans="1:2">
+    <row r="343" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>342</v>
       </c>
@@ -5620,7 +5688,7 @@
         <v>754</v>
       </c>
     </row>
-    <row r="344" spans="1:2">
+    <row r="344" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>343</v>
       </c>
@@ -5628,7 +5696,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="345" spans="1:2">
+    <row r="345" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>344</v>
       </c>
@@ -5636,7 +5704,7 @@
         <v>756</v>
       </c>
     </row>
-    <row r="346" spans="1:2">
+    <row r="346" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>345</v>
       </c>
@@ -5644,7 +5712,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="347" spans="1:2">
+    <row r="347" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>346</v>
       </c>
@@ -5652,7 +5720,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="348" spans="1:2">
+    <row r="348" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>347</v>
       </c>
@@ -5660,7 +5728,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="349" spans="1:2">
+    <row r="349" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>348</v>
       </c>
@@ -5668,7 +5736,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="350" spans="1:2">
+    <row r="350" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>349</v>
       </c>
@@ -5676,7 +5744,7 @@
         <v>761</v>
       </c>
     </row>
-    <row r="351" spans="1:2">
+    <row r="351" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>350</v>
       </c>
@@ -5684,7 +5752,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="352" spans="1:2">
+    <row r="352" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>351</v>
       </c>
@@ -5692,7 +5760,7 @@
         <v>763</v>
       </c>
     </row>
-    <row r="353" spans="1:2">
+    <row r="353" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>352</v>
       </c>
@@ -5700,7 +5768,7 @@
         <v>764</v>
       </c>
     </row>
-    <row r="354" spans="1:2">
+    <row r="354" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>353</v>
       </c>
@@ -5708,7 +5776,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="355" spans="1:2">
+    <row r="355" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>354</v>
       </c>
@@ -5716,7 +5784,7 @@
         <v>765</v>
       </c>
     </row>
-    <row r="356" spans="1:2">
+    <row r="356" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>355</v>
       </c>
@@ -5724,7 +5792,7 @@
         <v>766</v>
       </c>
     </row>
-    <row r="357" spans="1:2">
+    <row r="357" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>356</v>
       </c>
@@ -5732,7 +5800,7 @@
         <v>767</v>
       </c>
     </row>
-    <row r="358" spans="1:2">
+    <row r="358" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>357</v>
       </c>
@@ -5740,7 +5808,7 @@
         <v>768</v>
       </c>
     </row>
-    <row r="359" spans="1:2">
+    <row r="359" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>358</v>
       </c>
@@ -5748,7 +5816,7 @@
         <v>769</v>
       </c>
     </row>
-    <row r="360" spans="1:2">
+    <row r="360" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>359</v>
       </c>
@@ -5756,7 +5824,7 @@
         <v>770</v>
       </c>
     </row>
-    <row r="361" spans="1:2">
+    <row r="361" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>360</v>
       </c>
@@ -5764,7 +5832,7 @@
         <v>771</v>
       </c>
     </row>
-    <row r="362" spans="1:2">
+    <row r="362" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>361</v>
       </c>
@@ -5772,7 +5840,7 @@
         <v>772</v>
       </c>
     </row>
-    <row r="363" spans="1:2">
+    <row r="363" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>362</v>
       </c>
@@ -5780,7 +5848,7 @@
         <v>773</v>
       </c>
     </row>
-    <row r="364" spans="1:2">
+    <row r="364" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>363</v>
       </c>
@@ -5788,7 +5856,7 @@
         <v>774</v>
       </c>
     </row>
-    <row r="365" spans="1:2">
+    <row r="365" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>364</v>
       </c>
@@ -5796,7 +5864,7 @@
         <v>775</v>
       </c>
     </row>
-    <row r="366" spans="1:2">
+    <row r="366" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>365</v>
       </c>
@@ -5804,7 +5872,7 @@
         <v>776</v>
       </c>
     </row>
-    <row r="367" spans="1:2">
+    <row r="367" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>366</v>
       </c>
@@ -5812,7 +5880,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="368" spans="1:2">
+    <row r="368" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>367</v>
       </c>
@@ -5820,7 +5888,7 @@
         <v>778</v>
       </c>
     </row>
-    <row r="369" spans="1:2">
+    <row r="369" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>368</v>
       </c>
@@ -5828,7 +5896,7 @@
         <v>779</v>
       </c>
     </row>
-    <row r="370" spans="1:2">
+    <row r="370" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>369</v>
       </c>
@@ -5836,7 +5904,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="371" spans="1:2">
+    <row r="371" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>370</v>
       </c>
@@ -5844,7 +5912,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="372" spans="1:2">
+    <row r="372" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>371</v>
       </c>
@@ -5852,7 +5920,7 @@
         <v>782</v>
       </c>
     </row>
-    <row r="373" spans="1:2">
+    <row r="373" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>372</v>
       </c>
@@ -5860,7 +5928,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="374" spans="1:2">
+    <row r="374" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>373</v>
       </c>
@@ -5868,7 +5936,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="375" spans="1:2">
+    <row r="375" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>374</v>
       </c>
@@ -5876,7 +5944,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="376" spans="1:2">
+    <row r="376" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>375</v>
       </c>
@@ -5884,7 +5952,7 @@
         <v>785</v>
       </c>
     </row>
-    <row r="377" spans="1:2">
+    <row r="377" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>376</v>
       </c>
@@ -5892,7 +5960,7 @@
         <v>786</v>
       </c>
     </row>
-    <row r="378" spans="1:2">
+    <row r="378" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>377</v>
       </c>
@@ -5900,7 +5968,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="379" spans="1:2">
+    <row r="379" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>378</v>
       </c>
@@ -5908,7 +5976,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="380" spans="1:2">
+    <row r="380" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>379</v>
       </c>
@@ -5916,7 +5984,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="381" spans="1:2">
+    <row r="381" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>380</v>
       </c>
@@ -5924,7 +5992,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="382" spans="1:2">
+    <row r="382" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>381</v>
       </c>
@@ -5932,7 +6000,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="383" spans="1:2">
+    <row r="383" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>382</v>
       </c>
@@ -5940,7 +6008,7 @@
         <v>792</v>
       </c>
     </row>
-    <row r="384" spans="1:2">
+    <row r="384" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>383</v>
       </c>
@@ -5948,7 +6016,7 @@
         <v>793</v>
       </c>
     </row>
-    <row r="385" spans="1:2">
+    <row r="385" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>384</v>
       </c>
@@ -5956,7 +6024,7 @@
         <v>794</v>
       </c>
     </row>
-    <row r="386" spans="1:2">
+    <row r="386" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>385</v>
       </c>
@@ -5964,7 +6032,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="387" spans="1:2">
+    <row r="387" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>386</v>
       </c>
@@ -5972,7 +6040,7 @@
         <v>796</v>
       </c>
     </row>
-    <row r="388" spans="1:2">
+    <row r="388" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>387</v>
       </c>
@@ -5980,7 +6048,7 @@
         <v>797</v>
       </c>
     </row>
-    <row r="389" spans="1:2">
+    <row r="389" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>388</v>
       </c>
@@ -5988,7 +6056,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="390" spans="1:2">
+    <row r="390" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>138</v>
       </c>
@@ -5996,7 +6064,7 @@
         <v>799</v>
       </c>
     </row>
-    <row r="391" spans="1:2">
+    <row r="391" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>389</v>
       </c>
@@ -6004,7 +6072,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="392" spans="1:2">
+    <row r="392" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>390</v>
       </c>
@@ -6012,7 +6080,7 @@
         <v>801</v>
       </c>
     </row>
-    <row r="393" spans="1:2">
+    <row r="393" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>391</v>
       </c>
@@ -6020,7 +6088,7 @@
         <v>802</v>
       </c>
     </row>
-    <row r="394" spans="1:2">
+    <row r="394" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A394" t="s">
         <v>392</v>
       </c>
@@ -6028,7 +6096,7 @@
         <v>803</v>
       </c>
     </row>
-    <row r="395" spans="1:2">
+    <row r="395" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A395" t="s">
         <v>393</v>
       </c>
@@ -6036,7 +6104,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="396" spans="1:2">
+    <row r="396" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A396" t="s">
         <v>394</v>
       </c>
@@ -6044,7 +6112,7 @@
         <v>805</v>
       </c>
     </row>
-    <row r="397" spans="1:2">
+    <row r="397" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A397" t="s">
         <v>395</v>
       </c>
@@ -6052,7 +6120,7 @@
         <v>806</v>
       </c>
     </row>
-    <row r="398" spans="1:2">
+    <row r="398" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A398" t="s">
         <v>396</v>
       </c>
@@ -6060,7 +6128,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="399" spans="1:2">
+    <row r="399" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A399" t="s">
         <v>397</v>
       </c>
@@ -6068,7 +6136,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="400" spans="1:2">
+    <row r="400" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A400" t="s">
         <v>398</v>
       </c>
@@ -6076,7 +6144,7 @@
         <v>809</v>
       </c>
     </row>
-    <row r="401" spans="1:2">
+    <row r="401" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A401" t="s">
         <v>399</v>
       </c>
@@ -6084,7 +6152,7 @@
         <v>810</v>
       </c>
     </row>
-    <row r="402" spans="1:2">
+    <row r="402" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A402" t="s">
         <v>400</v>
       </c>
@@ -6092,7 +6160,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="403" spans="1:2">
+    <row r="403" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A403" t="s">
         <v>401</v>
       </c>
@@ -6100,7 +6168,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="404" spans="1:2">
+    <row r="404" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A404" t="s">
         <v>402</v>
       </c>
@@ -6108,7 +6176,7 @@
         <v>813</v>
       </c>
     </row>
-    <row r="405" spans="1:2">
+    <row r="405" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A405" t="s">
         <v>403</v>
       </c>
@@ -6116,7 +6184,7 @@
         <v>814</v>
       </c>
     </row>
-    <row r="406" spans="1:2">
+    <row r="406" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A406" t="s">
         <v>404</v>
       </c>
@@ -6124,7 +6192,7 @@
         <v>815</v>
       </c>
     </row>
-    <row r="407" spans="1:2">
+    <row r="407" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A407" t="s">
         <v>405</v>
       </c>
@@ -6132,7 +6200,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="408" spans="1:2">
+    <row r="408" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A408" t="s">
         <v>406</v>
       </c>
@@ -6140,7 +6208,7 @@
         <v>817</v>
       </c>
     </row>
-    <row r="409" spans="1:2">
+    <row r="409" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A409" t="s">
         <v>407</v>
       </c>
@@ -6148,7 +6216,7 @@
         <v>818</v>
       </c>
     </row>
-    <row r="410" spans="1:2">
+    <row r="410" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A410" t="s">
         <v>408</v>
       </c>
@@ -6156,7 +6224,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="411" spans="1:2">
+    <row r="411" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A411" t="s">
         <v>409</v>
       </c>
@@ -6164,7 +6232,7 @@
         <v>820</v>
       </c>
     </row>
-    <row r="412" spans="1:2">
+    <row r="412" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A412" t="s">
         <v>410</v>
       </c>
@@ -6172,7 +6240,7 @@
         <v>821</v>
       </c>
     </row>
-    <row r="413" spans="1:2">
+    <row r="413" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A413" t="s">
         <v>411</v>
       </c>
@@ -6180,7 +6248,7 @@
         <v>822</v>
       </c>
     </row>
-    <row r="414" spans="1:2">
+    <row r="414" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A414" t="s">
         <v>412</v>
       </c>
@@ -6188,7 +6256,7 @@
         <v>823</v>
       </c>
     </row>
-    <row r="415" spans="1:2">
+    <row r="415" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A415" t="s">
         <v>413</v>
       </c>
@@ -6196,7 +6264,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="416" spans="1:2">
+    <row r="416" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A416" t="s">
         <v>414</v>
       </c>
@@ -6204,7 +6272,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="417" spans="1:2">
+    <row r="417" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A417" t="s">
         <v>415</v>
       </c>
@@ -6212,7 +6280,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="418" spans="1:2">
+    <row r="418" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A418" t="s">
         <v>416</v>
       </c>
@@ -6220,7 +6288,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="419" spans="1:2">
+    <row r="419" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A419" t="s">
         <v>417</v>
       </c>
@@ -6228,7 +6296,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="420" spans="1:2">
+    <row r="420" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A420" t="s">
         <v>418</v>
       </c>
@@ -6236,7 +6304,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="421" spans="1:2">
+    <row r="421" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A421" t="s">
         <v>419</v>
       </c>
@@ -6244,7 +6312,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="422" spans="1:2">
+    <row r="422" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A422" t="s">
         <v>420</v>
       </c>
@@ -6252,7 +6320,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="423" spans="1:2">
+    <row r="423" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A423" t="s">
         <v>421</v>
       </c>
@@ -6260,12 +6328,28 @@
         <v>832</v>
       </c>
     </row>
-    <row r="424" spans="1:2">
+    <row r="424" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A424" t="s">
         <v>422</v>
       </c>
       <c r="B424" t="s">
         <v>460</v>
+      </c>
+    </row>
+    <row r="425" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A425" t="s">
+        <v>833</v>
+      </c>
+      <c r="B425" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="426" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A426" t="s">
+        <v>835</v>
+      </c>
+      <c r="B426" t="s">
+        <v>836</v>
       </c>
     </row>
   </sheetData>

</xml_diff>